<commit_message>
Kapitel 8 eliminiert und alles dahinter nach vorne gezogen
</commit_message>
<xml_diff>
--- a/Zeitaufteilung.xlsx
+++ b/Zeitaufteilung.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanner/Library/CloudStorage/Dropbox/geri/iSAQB/GREEN/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanner/curriculum-green/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57BD9792-7C5F-AB45-8485-5DC8B9A5221A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CFB0D8-3B66-1945-A89A-FF2C50E48AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="59260" yWindow="-13940" windowWidth="32180" windowHeight="20540" xr2:uid="{164985D6-E6B5-0E4B-A008-223BB3A35586}"/>
+    <workbookView xWindow="38140" yWindow="-13780" windowWidth="32180" windowHeight="20540" xr2:uid="{164985D6-E6B5-0E4B-A008-223BB3A35586}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>Skizzierung einer Architektur</t>
   </si>
   <si>
-    <t>Gesamtsumme</t>
-  </si>
-  <si>
     <t>Braucht Rechner</t>
   </si>
   <si>
@@ -103,6 +100,9 @@
   </si>
   <si>
     <t>Beispielhaft Messwerkzeuge ausprobieren, ggf. i.V.m. Softwareentwicklung</t>
+  </si>
+  <si>
+    <t>Summe</t>
   </si>
 </sst>
 </file>
@@ -495,21 +495,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42304E5D-7C16-2D47-80BB-73F55E94CA4E}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="57.5" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="60.33203125" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" customWidth="1"/>
+    <col min="5" max="5" width="60.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -520,29 +521,40 @@
         <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <f>+B2+C2</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <f t="shared" ref="D3:D12" si="0">+B3+C3</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -552,11 +564,15 @@
       <c r="C4">
         <v>30</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -566,22 +582,30 @@
       <c r="C5">
         <v>60</v>
       </c>
-      <c r="D5" t="s">
-        <v>21</v>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>135</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -591,13 +615,17 @@
       <c r="C7">
         <v>60</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="E7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2">
         <v>75</v>
@@ -605,30 +633,42 @@
       <c r="C8" s="2">
         <v>30</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>45</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12">
         <f>SUM(B2:B11)</f>
         <v>540</v>
@@ -637,29 +677,25 @@
         <f>SUM(C2:C11)</f>
         <v>180</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <f>+B12+C12</f>
+        <f>+D12</f>
         <v>720</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="C14">
+        <f>B14/60</f>
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
         <v>14</v>
-      </c>
-      <c r="B15">
-        <v>720</v>
-      </c>
-      <c r="C15">
-        <f>B15/60</f>
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Zeiten aktualisiert und in allen Kapiteln eingetragen, Gendern
</commit_message>
<xml_diff>
--- a/Zeitaufteilung.xlsx
+++ b/Zeitaufteilung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wanner/curriculum-green/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CFB0D8-3B66-1945-A89A-FF2C50E48AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD31E7E-BD06-D94B-97C9-AC4CDAA6AC99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38140" yWindow="-13780" windowWidth="32180" windowHeight="20540" xr2:uid="{164985D6-E6B5-0E4B-A008-223BB3A35586}"/>
+    <workbookView xWindow="80180" yWindow="-11360" windowWidth="35660" windowHeight="22440" xr2:uid="{164985D6-E6B5-0E4B-A008-223BB3A35586}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="2" r:id="rId1"/>
@@ -153,14 +153,18 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -498,203 +502,205 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.5" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" customWidth="1"/>
-    <col min="5" max="5" width="60.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>60</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="1">
+        <v>60</v>
+      </c>
+      <c r="D2" s="1">
         <f>+B2+C2</f>
         <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>60</v>
-      </c>
-      <c r="D3">
+      <c r="B3" s="1">
+        <v>60</v>
+      </c>
+      <c r="D3" s="1">
         <f t="shared" ref="D3:D12" si="0">+B3+C3</f>
         <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4">
         <v>45</v>
       </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="1">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
+        <v>90</v>
+      </c>
+      <c r="C5" s="1">
+        <v>60</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>150</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>75</v>
+      </c>
+      <c r="D6" s="1">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="4">
-        <v>75</v>
-      </c>
-      <c r="C5">
-        <v>60</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>135</v>
-      </c>
-      <c r="E5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>60</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>90</v>
       </c>
-      <c r="C7">
-        <v>60</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="1">
+        <v>60</v>
+      </c>
+      <c r="D7" s="1">
         <f t="shared" si="0"/>
         <v>150</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>75</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>30</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9">
-        <v>45</v>
-      </c>
-      <c r="D9">
+      <c r="B9" s="1">
+        <v>60</v>
+      </c>
+      <c r="D9" s="1">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10">
-        <v>30</v>
-      </c>
-      <c r="D10">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B12">
+      <c r="B12" s="1">
         <f>SUM(B2:B11)</f>
-        <v>540</v>
-      </c>
-      <c r="C12">
+        <v>555</v>
+      </c>
+      <c r="C12" s="1">
         <f>SUM(C2:C11)</f>
-        <v>180</v>
-      </c>
-      <c r="D12">
+        <v>165</v>
+      </c>
+      <c r="D12" s="1">
         <f t="shared" si="0"/>
         <v>720</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <f>+D12</f>
         <v>720</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <f>B14/60</f>
         <v>12</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>